<commit_message>
With validated picks from PDF
</commit_message>
<xml_diff>
--- a/nba-over-under-2021-2022/picks.xlsx
+++ b/nba-over-under-2021-2022/picks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chester/Desktop/Desktop - Chester’s MacBook Pro/ismayc.github.io/nba-over-under-2021-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E94867E3-5728-D947-912F-B4161DEC4D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{10DE97CC-68FB-1447-9E24-FBABCC242D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18900" windowHeight="23940" activeTab="1" xr2:uid="{C9BABCDB-CBFD-8A40-A903-BB9D75C68790}"/>
+    <workbookView xWindow="4220" yWindow="500" windowWidth="18900" windowHeight="23940" xr2:uid="{C9BABCDB-CBFD-8A40-A903-BB9D75C68790}"/>
   </bookViews>
   <sheets>
     <sheet name="picks" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="854" uniqueCount="56">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="885" uniqueCount="87">
   <si>
     <t>team</t>
   </si>
@@ -211,6 +211,99 @@
   </si>
   <si>
     <t>Dropdown</t>
+  </si>
+  <si>
+    <t>abbreviation</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>BKN</t>
+  </si>
+  <si>
+    <t>CHA</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>NYK</t>
+  </si>
+  <si>
+    <t>ORL</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>GSW</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>LAC</t>
+  </si>
+  <si>
+    <t>LAL</t>
+  </si>
+  <si>
+    <t>MEM</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>OKC</t>
+  </si>
+  <si>
+    <t>PHO</t>
+  </si>
+  <si>
+    <t>POR</t>
+  </si>
+  <si>
+    <t>SAC</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t>UTA</t>
   </si>
 </sst>
 </file>
@@ -572,8 +665,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A42A21-1461-8645-BA2E-931098BDDD56}">
   <dimension ref="A1:E241"/>
   <sheetViews>
-    <sheetView topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="E198" sqref="E198"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2765,7 +2858,7 @@
       </c>
       <c r="B122" t="str">
         <f>VLOOKUP(A122,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C122" t="s">
         <v>6</v>
@@ -2783,7 +2876,7 @@
       </c>
       <c r="B123" t="str">
         <f>VLOOKUP(A123,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C123" t="s">
         <v>3</v>
@@ -2801,7 +2894,7 @@
       </c>
       <c r="B124" t="str">
         <f>VLOOKUP(A124,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C124" t="s">
         <v>4</v>
@@ -2819,7 +2912,7 @@
       </c>
       <c r="B125" t="str">
         <f>VLOOKUP(A125,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C125" t="s">
         <v>5</v>
@@ -2837,7 +2930,7 @@
       </c>
       <c r="B126" t="str">
         <f>VLOOKUP(A126,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C126" t="s">
         <v>10</v>
@@ -2855,7 +2948,7 @@
       </c>
       <c r="B127" t="str">
         <f>VLOOKUP(A127,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C127" t="s">
         <v>7</v>
@@ -2873,7 +2966,7 @@
       </c>
       <c r="B128" t="str">
         <f>VLOOKUP(A128,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
@@ -2891,7 +2984,7 @@
       </c>
       <c r="B129" t="str">
         <f>VLOOKUP(A129,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -2909,7 +3002,7 @@
       </c>
       <c r="B130" t="str">
         <f>VLOOKUP(A130,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C130" t="s">
         <v>6</v>
@@ -2927,7 +3020,7 @@
       </c>
       <c r="B131" t="str">
         <f>VLOOKUP(A131,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C131" t="s">
         <v>3</v>
@@ -2945,7 +3038,7 @@
       </c>
       <c r="B132" t="str">
         <f>VLOOKUP(A132,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C132" t="s">
         <v>4</v>
@@ -2963,7 +3056,7 @@
       </c>
       <c r="B133" t="str">
         <f>VLOOKUP(A133,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C133" t="s">
         <v>5</v>
@@ -2981,7 +3074,7 @@
       </c>
       <c r="B134" t="str">
         <f>VLOOKUP(A134,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C134" t="s">
         <v>10</v>
@@ -2999,7 +3092,7 @@
       </c>
       <c r="B135" t="str">
         <f>VLOOKUP(A135,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C135" t="s">
         <v>7</v>
@@ -3017,7 +3110,7 @@
       </c>
       <c r="B136" t="str">
         <f>VLOOKUP(A136,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
@@ -3035,7 +3128,7 @@
       </c>
       <c r="B137" t="str">
         <f>VLOOKUP(A137,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -3053,7 +3146,7 @@
       </c>
       <c r="B138" t="str">
         <f>VLOOKUP(A138,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C138" t="s">
         <v>6</v>
@@ -3071,7 +3164,7 @@
       </c>
       <c r="B139" t="str">
         <f>VLOOKUP(A139,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C139" t="s">
         <v>3</v>
@@ -3089,7 +3182,7 @@
       </c>
       <c r="B140" t="str">
         <f>VLOOKUP(A140,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C140" t="s">
         <v>4</v>
@@ -3107,7 +3200,7 @@
       </c>
       <c r="B141" t="str">
         <f>VLOOKUP(A141,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C141" t="s">
         <v>5</v>
@@ -3125,7 +3218,7 @@
       </c>
       <c r="B142" t="str">
         <f>VLOOKUP(A142,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C142" t="s">
         <v>10</v>
@@ -3143,7 +3236,7 @@
       </c>
       <c r="B143" t="str">
         <f>VLOOKUP(A143,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C143" t="s">
         <v>7</v>
@@ -3161,7 +3254,7 @@
       </c>
       <c r="B144" t="str">
         <f>VLOOKUP(A144,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C144" t="s">
         <v>9</v>
@@ -3179,7 +3272,7 @@
       </c>
       <c r="B145" t="str">
         <f>VLOOKUP(A145,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C145" t="s">
         <v>8</v>
@@ -3197,7 +3290,7 @@
       </c>
       <c r="B146" t="str">
         <f>VLOOKUP(A146,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
@@ -3215,7 +3308,7 @@
       </c>
       <c r="B147" t="str">
         <f>VLOOKUP(A147,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C147" t="s">
         <v>3</v>
@@ -3233,7 +3326,7 @@
       </c>
       <c r="B148" t="str">
         <f>VLOOKUP(A148,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C148" t="s">
         <v>4</v>
@@ -3251,7 +3344,7 @@
       </c>
       <c r="B149" t="str">
         <f>VLOOKUP(A149,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C149" t="s">
         <v>5</v>
@@ -3269,7 +3362,7 @@
       </c>
       <c r="B150" t="str">
         <f>VLOOKUP(A150,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C150" t="s">
         <v>10</v>
@@ -3287,7 +3380,7 @@
       </c>
       <c r="B151" t="str">
         <f>VLOOKUP(A151,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C151" t="s">
         <v>7</v>
@@ -3305,7 +3398,7 @@
       </c>
       <c r="B152" t="str">
         <f>VLOOKUP(A152,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C152" t="s">
         <v>9</v>
@@ -3323,7 +3416,7 @@
       </c>
       <c r="B153" t="str">
         <f>VLOOKUP(A153,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C153" t="s">
         <v>8</v>
@@ -3341,7 +3434,7 @@
       </c>
       <c r="B154" t="str">
         <f>VLOOKUP(A154,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C154" t="s">
         <v>6</v>
@@ -3359,7 +3452,7 @@
       </c>
       <c r="B155" t="str">
         <f>VLOOKUP(A155,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C155" t="s">
         <v>3</v>
@@ -3377,7 +3470,7 @@
       </c>
       <c r="B156" t="str">
         <f>VLOOKUP(A156,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C156" t="s">
         <v>4</v>
@@ -3395,7 +3488,7 @@
       </c>
       <c r="B157" t="str">
         <f>VLOOKUP(A157,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C157" t="s">
         <v>5</v>
@@ -3413,7 +3506,7 @@
       </c>
       <c r="B158" t="str">
         <f>VLOOKUP(A158,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C158" t="s">
         <v>10</v>
@@ -3431,7 +3524,7 @@
       </c>
       <c r="B159" t="str">
         <f>VLOOKUP(A159,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C159" t="s">
         <v>7</v>
@@ -3449,7 +3542,7 @@
       </c>
       <c r="B160" t="str">
         <f>VLOOKUP(A160,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C160" t="s">
         <v>9</v>
@@ -3467,7 +3560,7 @@
       </c>
       <c r="B161" t="str">
         <f>VLOOKUP(A161,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C161" t="s">
         <v>8</v>
@@ -3485,7 +3578,7 @@
       </c>
       <c r="B162" t="str">
         <f>VLOOKUP(A162,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C162" t="s">
         <v>6</v>
@@ -3503,7 +3596,7 @@
       </c>
       <c r="B163" t="str">
         <f>VLOOKUP(A163,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C163" t="s">
         <v>3</v>
@@ -3521,7 +3614,7 @@
       </c>
       <c r="B164" t="str">
         <f>VLOOKUP(A164,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C164" t="s">
         <v>4</v>
@@ -3539,7 +3632,7 @@
       </c>
       <c r="B165" t="str">
         <f>VLOOKUP(A165,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C165" t="s">
         <v>5</v>
@@ -3557,7 +3650,7 @@
       </c>
       <c r="B166" t="str">
         <f>VLOOKUP(A166,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C166" t="s">
         <v>10</v>
@@ -3575,7 +3668,7 @@
       </c>
       <c r="B167" t="str">
         <f>VLOOKUP(A167,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C167" t="s">
         <v>7</v>
@@ -3593,7 +3686,7 @@
       </c>
       <c r="B168" t="str">
         <f>VLOOKUP(A168,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C168" t="s">
         <v>9</v>
@@ -3611,7 +3704,7 @@
       </c>
       <c r="B169" t="str">
         <f>VLOOKUP(A169,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C169" t="s">
         <v>8</v>
@@ -3629,7 +3722,7 @@
       </c>
       <c r="B170" t="str">
         <f>VLOOKUP(A170,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C170" t="s">
         <v>6</v>
@@ -3647,7 +3740,7 @@
       </c>
       <c r="B171" t="str">
         <f>VLOOKUP(A171,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C171" t="s">
         <v>3</v>
@@ -3665,7 +3758,7 @@
       </c>
       <c r="B172" t="str">
         <f>VLOOKUP(A172,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C172" t="s">
         <v>4</v>
@@ -3683,7 +3776,7 @@
       </c>
       <c r="B173" t="str">
         <f>VLOOKUP(A173,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C173" t="s">
         <v>5</v>
@@ -3701,7 +3794,7 @@
       </c>
       <c r="B174" t="str">
         <f>VLOOKUP(A174,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C174" t="s">
         <v>10</v>
@@ -3719,7 +3812,7 @@
       </c>
       <c r="B175" t="str">
         <f>VLOOKUP(A175,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C175" t="s">
         <v>7</v>
@@ -3737,7 +3830,7 @@
       </c>
       <c r="B176" t="str">
         <f>VLOOKUP(A176,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C176" t="s">
         <v>9</v>
@@ -3755,7 +3848,7 @@
       </c>
       <c r="B177" t="str">
         <f>VLOOKUP(A177,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C177" t="s">
         <v>8</v>
@@ -3773,7 +3866,7 @@
       </c>
       <c r="B178" t="str">
         <f>VLOOKUP(A178,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C178" t="s">
         <v>6</v>
@@ -3791,7 +3884,7 @@
       </c>
       <c r="B179" t="str">
         <f>VLOOKUP(A179,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C179" t="s">
         <v>3</v>
@@ -3809,7 +3902,7 @@
       </c>
       <c r="B180" t="str">
         <f>VLOOKUP(A180,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C180" t="s">
         <v>4</v>
@@ -3827,7 +3920,7 @@
       </c>
       <c r="B181" t="str">
         <f>VLOOKUP(A181,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C181" t="s">
         <v>5</v>
@@ -3845,7 +3938,7 @@
       </c>
       <c r="B182" t="str">
         <f>VLOOKUP(A182,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C182" t="s">
         <v>10</v>
@@ -3863,7 +3956,7 @@
       </c>
       <c r="B183" t="str">
         <f>VLOOKUP(A183,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C183" t="s">
         <v>7</v>
@@ -3881,7 +3974,7 @@
       </c>
       <c r="B184" t="str">
         <f>VLOOKUP(A184,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C184" t="s">
         <v>9</v>
@@ -3899,7 +3992,7 @@
       </c>
       <c r="B185" t="str">
         <f>VLOOKUP(A185,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C185" t="s">
         <v>8</v>
@@ -3917,7 +4010,7 @@
       </c>
       <c r="B186" t="str">
         <f>VLOOKUP(A186,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C186" t="s">
         <v>6</v>
@@ -3935,7 +4028,7 @@
       </c>
       <c r="B187" t="str">
         <f>VLOOKUP(A187,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C187" t="s">
         <v>3</v>
@@ -3953,7 +4046,7 @@
       </c>
       <c r="B188" t="str">
         <f>VLOOKUP(A188,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C188" t="s">
         <v>4</v>
@@ -3971,7 +4064,7 @@
       </c>
       <c r="B189" t="str">
         <f>VLOOKUP(A189,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C189" t="s">
         <v>5</v>
@@ -3989,7 +4082,7 @@
       </c>
       <c r="B190" t="str">
         <f>VLOOKUP(A190,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C190" t="s">
         <v>10</v>
@@ -4007,7 +4100,7 @@
       </c>
       <c r="B191" t="str">
         <f>VLOOKUP(A191,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C191" t="s">
         <v>7</v>
@@ -4025,7 +4118,7 @@
       </c>
       <c r="B192" t="str">
         <f>VLOOKUP(A192,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C192" t="s">
         <v>9</v>
@@ -4043,7 +4136,7 @@
       </c>
       <c r="B193" t="str">
         <f>VLOOKUP(A193,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C193" t="s">
         <v>8</v>
@@ -4061,7 +4154,7 @@
       </c>
       <c r="B194" t="str">
         <f>VLOOKUP(A194,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C194" t="s">
         <v>6</v>
@@ -4079,7 +4172,7 @@
       </c>
       <c r="B195" t="str">
         <f>VLOOKUP(A195,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C195" t="s">
         <v>3</v>
@@ -4097,7 +4190,7 @@
       </c>
       <c r="B196" t="str">
         <f>VLOOKUP(A196,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C196" t="s">
         <v>4</v>
@@ -4115,7 +4208,7 @@
       </c>
       <c r="B197" t="str">
         <f>VLOOKUP(A197,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C197" t="s">
         <v>5</v>
@@ -4133,7 +4226,7 @@
       </c>
       <c r="B198" t="str">
         <f>VLOOKUP(A198,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C198" t="s">
         <v>10</v>
@@ -4142,7 +4235,7 @@
         <v>7</v>
       </c>
       <c r="E198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -4151,7 +4244,7 @@
       </c>
       <c r="B199" t="str">
         <f>VLOOKUP(A199,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C199" t="s">
         <v>7</v>
@@ -4169,7 +4262,7 @@
       </c>
       <c r="B200" t="str">
         <f>VLOOKUP(A200,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C200" t="s">
         <v>9</v>
@@ -4187,7 +4280,7 @@
       </c>
       <c r="B201" t="str">
         <f>VLOOKUP(A201,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C201" t="s">
         <v>8</v>
@@ -4205,7 +4298,7 @@
       </c>
       <c r="B202" t="str">
         <f>VLOOKUP(A202,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C202" t="s">
         <v>6</v>
@@ -4223,7 +4316,7 @@
       </c>
       <c r="B203" t="str">
         <f>VLOOKUP(A203,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C203" t="s">
         <v>3</v>
@@ -4241,7 +4334,7 @@
       </c>
       <c r="B204" t="str">
         <f>VLOOKUP(A204,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C204" t="s">
         <v>4</v>
@@ -4259,7 +4352,7 @@
       </c>
       <c r="B205" t="str">
         <f>VLOOKUP(A205,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C205" t="s">
         <v>5</v>
@@ -4277,7 +4370,7 @@
       </c>
       <c r="B206" t="str">
         <f>VLOOKUP(A206,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C206" t="s">
         <v>10</v>
@@ -4295,7 +4388,7 @@
       </c>
       <c r="B207" t="str">
         <f>VLOOKUP(A207,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C207" t="s">
         <v>7</v>
@@ -4313,7 +4406,7 @@
       </c>
       <c r="B208" t="str">
         <f>VLOOKUP(A208,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C208" t="s">
         <v>9</v>
@@ -4331,7 +4424,7 @@
       </c>
       <c r="B209" t="str">
         <f>VLOOKUP(A209,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C209" t="s">
         <v>8</v>
@@ -4349,7 +4442,7 @@
       </c>
       <c r="B210" t="str">
         <f>VLOOKUP(A210,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C210" t="s">
         <v>6</v>
@@ -4367,7 +4460,7 @@
       </c>
       <c r="B211" t="str">
         <f>VLOOKUP(A211,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C211" t="s">
         <v>3</v>
@@ -4385,7 +4478,7 @@
       </c>
       <c r="B212" t="str">
         <f>VLOOKUP(A212,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C212" t="s">
         <v>4</v>
@@ -4403,7 +4496,7 @@
       </c>
       <c r="B213" t="str">
         <f>VLOOKUP(A213,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C213" t="s">
         <v>5</v>
@@ -4421,7 +4514,7 @@
       </c>
       <c r="B214" t="str">
         <f>VLOOKUP(A214,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C214" t="s">
         <v>10</v>
@@ -4439,7 +4532,7 @@
       </c>
       <c r="B215" t="str">
         <f>VLOOKUP(A215,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C215" t="s">
         <v>7</v>
@@ -4457,7 +4550,7 @@
       </c>
       <c r="B216" t="str">
         <f>VLOOKUP(A216,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C216" t="s">
         <v>9</v>
@@ -4475,7 +4568,7 @@
       </c>
       <c r="B217" t="str">
         <f>VLOOKUP(A217,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C217" t="s">
         <v>8</v>
@@ -4493,7 +4586,7 @@
       </c>
       <c r="B218" t="str">
         <f>VLOOKUP(A218,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C218" t="s">
         <v>6</v>
@@ -4511,7 +4604,7 @@
       </c>
       <c r="B219" t="str">
         <f>VLOOKUP(A219,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C219" t="s">
         <v>3</v>
@@ -4529,7 +4622,7 @@
       </c>
       <c r="B220" t="str">
         <f>VLOOKUP(A220,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C220" t="s">
         <v>4</v>
@@ -4547,7 +4640,7 @@
       </c>
       <c r="B221" t="str">
         <f>VLOOKUP(A221,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C221" t="s">
         <v>5</v>
@@ -4565,7 +4658,7 @@
       </c>
       <c r="B222" t="str">
         <f>VLOOKUP(A222,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C222" t="s">
         <v>10</v>
@@ -4583,7 +4676,7 @@
       </c>
       <c r="B223" t="str">
         <f>VLOOKUP(A223,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C223" t="s">
         <v>7</v>
@@ -4601,7 +4694,7 @@
       </c>
       <c r="B224" t="str">
         <f>VLOOKUP(A224,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C224" t="s">
         <v>9</v>
@@ -4619,7 +4712,7 @@
       </c>
       <c r="B225" t="str">
         <f>VLOOKUP(A225,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C225" t="s">
         <v>8</v>
@@ -4637,7 +4730,7 @@
       </c>
       <c r="B226" t="str">
         <f>VLOOKUP(A226,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C226" t="s">
         <v>6</v>
@@ -4655,7 +4748,7 @@
       </c>
       <c r="B227" t="str">
         <f>VLOOKUP(A227,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C227" t="s">
         <v>3</v>
@@ -4673,7 +4766,7 @@
       </c>
       <c r="B228" t="str">
         <f>VLOOKUP(A228,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C228" t="s">
         <v>4</v>
@@ -4691,7 +4784,7 @@
       </c>
       <c r="B229" t="str">
         <f>VLOOKUP(A229,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C229" t="s">
         <v>5</v>
@@ -4709,7 +4802,7 @@
       </c>
       <c r="B230" t="str">
         <f>VLOOKUP(A230,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C230" t="s">
         <v>10</v>
@@ -4727,7 +4820,7 @@
       </c>
       <c r="B231" t="str">
         <f>VLOOKUP(A231,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C231" t="s">
         <v>7</v>
@@ -4745,7 +4838,7 @@
       </c>
       <c r="B232" t="str">
         <f>VLOOKUP(A232,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C232" t="s">
         <v>9</v>
@@ -4763,13 +4856,13 @@
       </c>
       <c r="B233" t="str">
         <f>VLOOKUP(A233,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C233" t="s">
         <v>8</v>
       </c>
       <c r="D233">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E233" t="s">
         <v>14</v>
@@ -4781,7 +4874,7 @@
       </c>
       <c r="B234" t="str">
         <f>VLOOKUP(A234,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C234" t="s">
         <v>6</v>
@@ -4799,7 +4892,7 @@
       </c>
       <c r="B235" t="str">
         <f>VLOOKUP(A235,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C235" t="s">
         <v>3</v>
@@ -4817,7 +4910,7 @@
       </c>
       <c r="B236" t="str">
         <f>VLOOKUP(A236,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C236" t="s">
         <v>4</v>
@@ -4835,7 +4928,7 @@
       </c>
       <c r="B237" t="str">
         <f>VLOOKUP(A237,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C237" t="s">
         <v>5</v>
@@ -4853,7 +4946,7 @@
       </c>
       <c r="B238" t="str">
         <f>VLOOKUP(A238,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C238" t="s">
         <v>10</v>
@@ -4871,7 +4964,7 @@
       </c>
       <c r="B239" t="str">
         <f>VLOOKUP(A239,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C239" t="s">
         <v>7</v>
@@ -4889,7 +4982,7 @@
       </c>
       <c r="B240" t="str">
         <f>VLOOKUP(A240,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C240" t="s">
         <v>9</v>
@@ -4907,7 +5000,7 @@
       </c>
       <c r="B241" t="str">
         <f>VLOOKUP(A241,meta!$A$2:$C$31, 2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C241" t="s">
         <v>8</v>
@@ -4945,7 +5038,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCAFC27-68EA-F14B-9842-E64C61A112DD}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -5152,7 +5245,7 @@
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP(A17,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C17">
         <v>48.5</v>
@@ -5164,7 +5257,7 @@
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(A18,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C18">
         <v>49.5</v>
@@ -5176,7 +5269,7 @@
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP(A19,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C19">
         <v>48.5</v>
@@ -5188,7 +5281,7 @@
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(A20,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C20">
         <v>22.5</v>
@@ -5200,7 +5293,7 @@
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(A21,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C21">
         <v>44.5</v>
@@ -5212,7 +5305,7 @@
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(A22,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C22">
         <v>52.5</v>
@@ -5224,7 +5317,7 @@
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(A23,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C23">
         <v>41.5</v>
@@ -5236,7 +5329,7 @@
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP(A24,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C24">
         <v>31.5</v>
@@ -5248,7 +5341,7 @@
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP(A25,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C25">
         <v>37.5</v>
@@ -5260,7 +5353,7 @@
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP(A26,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C26">
         <v>22.5</v>
@@ -5272,7 +5365,7 @@
       </c>
       <c r="B27" t="str">
         <f>VLOOKUP(A27,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C27">
         <v>51.5</v>
@@ -5284,7 +5377,7 @@
       </c>
       <c r="B28" t="str">
         <f>VLOOKUP(A28,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C28">
         <v>43.5</v>
@@ -5296,7 +5389,7 @@
       </c>
       <c r="B29" t="str">
         <f>VLOOKUP(A29,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C29">
         <v>35.5</v>
@@ -5308,7 +5401,7 @@
       </c>
       <c r="B30" t="str">
         <f>VLOOKUP(A30,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C30">
         <v>33.5</v>
@@ -5320,7 +5413,7 @@
       </c>
       <c r="B31" t="str">
         <f>VLOOKUP(A31,meta!$A$2:$C$31,2)</f>
-        <v>West</v>
+        <v>East</v>
       </c>
       <c r="C31">
         <v>54.5</v>
@@ -5337,10 +5430,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2645E3-9323-794D-9317-15824D639067}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="A2:C31"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5348,7 +5441,7 @@
     <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5358,8 +5451,11 @@
       <c r="C1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -5369,8 +5465,11 @@
       <c r="C2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -5380,8 +5479,11 @@
       <c r="C3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -5391,8 +5493,11 @@
       <c r="C4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -5402,8 +5507,11 @@
       <c r="C5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -5413,8 +5521,11 @@
       <c r="C6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -5424,142 +5535,181 @@
       <c r="C7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>46</v>
       </c>
       <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
       <c r="C18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
@@ -5567,132 +5717,168 @@
       <c r="C20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
       </c>
       <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
         <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>47</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
+      <c r="D31" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C31">
+    <sortCondition ref="B2:B31"/>
     <sortCondition ref="A2:A31"/>
-    <sortCondition ref="B2:B31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>